<commit_message>
loop fix for child entries
</commit_message>
<xml_diff>
--- a/samplefile/kfk.xlsx
+++ b/samplefile/kfk.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anand/Documents/sayansi/workspaces/condaws/exceljson/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anand/Documents/sayansi/workspaces/condaws/xlsx-json/samplefile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA884987-CDBF-CC45-AADD-5E0BA0BC0C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B7BFA6-850B-4444-A5B0-BCF22C4F9F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{54062B5B-119E-BD4B-B3A8-E27F027BEEC4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
   <si>
     <t>Source Topic</t>
   </si>
@@ -240,6 +240,15 @@
   </si>
   <si>
     <t>Source To Target Mapping/Transformation Logic</t>
+  </si>
+  <si>
+    <t>Zenga</t>
+  </si>
+  <si>
+    <t>RollaZenga</t>
+  </si>
+  <si>
+    <t>RollaZenga File</t>
   </si>
 </sst>
 </file>
@@ -691,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2EE713F-F4D0-1D4B-B856-52E62332C59B}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -870,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="1" t="str">
-        <f t="shared" ref="N4:N14" si="0">"This Is "&amp;I4&amp;" "&amp;J4&amp;" field"</f>
+        <f t="shared" ref="N4:N15" si="0">"This Is "&amp;I4&amp;" "&amp;J4&amp;" field"</f>
         <v>This Is MARS.SUN MARS.SUNname field</v>
       </c>
       <c r="O4" s="1"/>
@@ -904,7 +913,7 @@
         <v>16</v>
       </c>
       <c r="J5" s="1" t="str">
-        <f t="shared" ref="J5:J14" si="1">I5&amp;""&amp;"name"</f>
+        <f>I5&amp;""&amp;"name"</f>
         <v>MARS.MOONname</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -951,7 +960,7 @@
         <v>17</v>
       </c>
       <c r="J6" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J5:J15" si="1">I6&amp;""&amp;"name"</f>
         <v>MARS.EARTHname</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -1356,12 +1365,20 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Zenganame</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+      <c r="N15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>This Is Zenga Zenganame field</v>
+      </c>
       <c r="O15" s="1"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -1373,12 +1390,18 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="I16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
+      <c r="N16" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix for varius types
</commit_message>
<xml_diff>
--- a/samplefile/kfk.xlsx
+++ b/samplefile/kfk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anand/Documents/sayansi/workspaces/condaws/xlsx-json/samplefile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B7BFA6-850B-4444-A5B0-BCF22C4F9F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217AFCE9-C759-D74E-86B6-07070453164A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{54062B5B-119E-BD4B-B3A8-E27F027BEEC4}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="19400" xr2:uid="{54062B5B-119E-BD4B-B3A8-E27F027BEEC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Attribute Name</t>
   </si>
   <si>
-    <t>Source To Target Mapping.Transformation Logic</t>
-  </si>
-  <si>
     <t>Topc</t>
   </si>
   <si>
@@ -62,15 +59,9 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Source: Kafka</t>
-  </si>
-  <si>
     <t>Middleware</t>
   </si>
   <si>
-    <t>Target:FINAL Product Topic</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -249,6 +240,15 @@
   </si>
   <si>
     <t>RollaZenga File</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>Source: System</t>
+  </si>
+  <si>
+    <t>Target:System</t>
   </si>
 </sst>
 </file>
@@ -700,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2EE713F-F4D0-1D4B-B856-52E62332C59B}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -723,7 +723,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -731,10 +731,10 @@
       <c r="E1" s="7"/>
       <c r="F1" s="8"/>
       <c r="G1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -754,54 +754,54 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1">
         <v>3</v>
@@ -810,20 +810,20 @@
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J3" s="1" t="str">
         <f>I3&amp;""&amp;"name"</f>
         <v>MARSname</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="L3" s="1">
         <v>3</v>
@@ -839,16 +839,16 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E4" s="1">
         <v>18</v>
@@ -857,20 +857,20 @@
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="J4" s="1" t="str">
         <f>I4&amp;""&amp;"name"</f>
         <v>MARS.SUNname</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L4" s="1">
         <v>18</v>
@@ -886,16 +886,16 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1">
         <v>120</v>
@@ -904,20 +904,20 @@
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="J5" s="1" t="str">
         <f>I5&amp;""&amp;"name"</f>
         <v>MARS.MOONname</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="L5" s="1">
         <v>120</v>
@@ -933,16 +933,16 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1">
         <v>22</v>
@@ -951,20 +951,20 @@
         <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J6" s="1" t="str">
         <f t="shared" ref="J5:J15" si="1">I6&amp;""&amp;"name"</f>
         <v>MARS.EARTHname</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="L6" s="1">
         <v>22</v>
@@ -980,16 +980,16 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E7" s="1">
         <v>40</v>
@@ -998,20 +998,20 @@
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J7" s="1" t="str">
         <f t="shared" si="1"/>
         <v>MARS.EARTH.PLANETname</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L7" s="1">
         <v>40</v>
@@ -1027,16 +1027,16 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1">
         <v>10</v>
@@ -1045,20 +1045,20 @@
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J8" s="1" t="str">
         <f t="shared" si="1"/>
         <v>MARS.EARTH.SATALITEname</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="L8" s="1">
         <v>10</v>
@@ -1074,16 +1074,16 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1">
         <v>10</v>
@@ -1092,20 +1092,20 @@
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J9" s="1" t="str">
         <f t="shared" si="1"/>
         <v>MARS.SOLARname</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="L9" s="1">
         <v>10</v>
@@ -1121,16 +1121,16 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E10" s="1">
         <v>60</v>
@@ -1139,20 +1139,20 @@
         <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J10" s="1" t="str">
         <f t="shared" si="1"/>
         <v>MARS.SOLAR.BLAKHOLEname</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L10" s="1">
         <v>60</v>
@@ -1168,16 +1168,16 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E11" s="1">
         <v>10</v>
@@ -1186,20 +1186,20 @@
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J11" s="1" t="str">
         <f t="shared" si="1"/>
         <v>MARS.UNIVERSEname</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="L11" s="1">
         <v>10</v>
@@ -1215,16 +1215,16 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E12" s="1">
         <v>10</v>
@@ -1233,20 +1233,20 @@
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J12" s="1" t="str">
         <f t="shared" si="1"/>
         <v>MARS.UNIVERSE.GALAXYname</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="L12" s="1">
         <v>10</v>
@@ -1262,16 +1262,16 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E13" s="1">
         <v>220</v>
@@ -1280,20 +1280,20 @@
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J13" s="1" t="str">
         <f t="shared" si="1"/>
         <v>MARS.UNIVERSE.CENTERPTname</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L13" s="1">
         <v>220</v>
@@ -1306,21 +1306,21 @@
         <v>This Is MARS.UNIVERSE.CENTERPT MARS.UNIVERSE.CENTERPTname field</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E14" s="1">
         <v>10</v>
@@ -1329,20 +1329,20 @@
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J14" s="1" t="str">
         <f t="shared" si="1"/>
         <v>MARS.UNIVERSE.CENTERPT.HOLEname</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="L14" s="1">
         <v>10</v>
@@ -1366,7 +1366,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J15" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1391,16 +1391,16 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="O16" s="1"/>
     </row>
@@ -1489,7 +1489,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
@@ -1498,7 +1498,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -1516,7 +1516,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
@@ -1570,7 +1570,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
@@ -1579,7 +1579,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
min max fix and new line string fix
</commit_message>
<xml_diff>
--- a/samplefile/kfk.xlsx
+++ b/samplefile/kfk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anand/Documents/sayansi/workspaces/condaws/xlsx-json/samplefile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217AFCE9-C759-D74E-86B6-07070453164A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459E6EED-23F2-3149-A4A3-ADA000ADCACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="19400" xr2:uid="{54062B5B-119E-BD4B-B3A8-E27F027BEEC4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{54062B5B-119E-BD4B-B3A8-E27F027BEEC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="126">
   <si>
     <t>Source Topic</t>
   </si>
@@ -230,9 +230,6 @@
     <t>Decimal</t>
   </si>
   <si>
-    <t>Source To Target Mapping/Transformation Logic</t>
-  </si>
-  <si>
     <t>Zenga</t>
   </si>
   <si>
@@ -249,13 +246,182 @@
   </si>
   <si>
     <t>Target:System</t>
+  </si>
+  <si>
+    <t>This is MarName 
+and this is second line</t>
+  </si>
+  <si>
+    <t>components</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>transitions</t>
+  </si>
+  <si>
+    <t>uiapp</t>
+  </si>
+  <si>
+    <t>uimodule</t>
+  </si>
+  <si>
+    <t>uipage</t>
+  </si>
+  <si>
+    <t>componenttype</t>
+  </si>
+  <si>
+    <t>actiontype</t>
+  </si>
+  <si>
+    <t>transitiontype</t>
+  </si>
+  <si>
+    <t>objectid</t>
+  </si>
+  <si>
+    <t>uid</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>decisions</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>classes</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>transition</t>
+  </si>
+  <si>
+    <t>array[transition]</t>
+  </si>
+  <si>
+    <t>array[action]</t>
+  </si>
+  <si>
+    <t>actions</t>
+  </si>
+  <si>
+    <t>array[class]</t>
+  </si>
+  <si>
+    <t>inlinestyle</t>
+  </si>
+  <si>
+    <t>workflows</t>
+  </si>
+  <si>
+    <t>array[workflow]</t>
+  </si>
+  <si>
+    <t>workflow</t>
+  </si>
+  <si>
+    <t>icons</t>
+  </si>
+  <si>
+    <t>events</t>
+  </si>
+  <si>
+    <t>array[string]</t>
+  </si>
+  <si>
+    <t>array[event]</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>childrens</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>attributes</t>
+  </si>
+  <si>
+    <t>object&lt;component&gt;</t>
+  </si>
+  <si>
+    <t>array[component]</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>alt</t>
+  </si>
+  <si>
+    <t>src</t>
+  </si>
+  <si>
+    <t>href</t>
+  </si>
+  <si>
+    <t>lang</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>map[string,string]</t>
+  </si>
+  <si>
+    <t>rendermap</t>
+  </si>
+  <si>
+    <t>object&lt;attributes&gt;</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>object&lt;componenttype&gt;</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>double</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -277,8 +443,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,8 +477,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -364,17 +550,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -384,6 +588,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2EE713F-F4D0-1D4B-B856-52E62332C59B}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -722,19 +929,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="8"/>
+      <c r="A1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
       <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -763,7 +970,7 @@
         <v>63</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>3</v>
@@ -790,7 +997,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -823,17 +1030,16 @@
         <v>MARSname</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="L3" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M3" s="1">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1" t="str">
-        <f>"This Is "&amp;I3&amp;" "&amp;J3&amp;" field"</f>
-        <v>This Is MARS MARSname field</v>
+        <v>2</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="O3" s="1"/>
     </row>
@@ -873,7 +1079,7 @@
         <v>59</v>
       </c>
       <c r="L4" s="1">
-        <v>18</v>
+        <v>550</v>
       </c>
       <c r="M4" s="1">
         <v>0</v>
@@ -920,7 +1126,7 @@
         <v>8</v>
       </c>
       <c r="L5" s="1">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
@@ -960,14 +1166,14 @@
         <v>14</v>
       </c>
       <c r="J6" s="1" t="str">
-        <f t="shared" ref="J5:J15" si="1">I6&amp;""&amp;"name"</f>
+        <f t="shared" ref="J6:J15" si="1">I6&amp;""&amp;"name"</f>
         <v>MARS.EARTHname</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>8</v>
+        <v>124</v>
       </c>
       <c r="L6" s="1">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
@@ -1366,14 +1572,18 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J15" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Zenganame</v>
       </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L15" s="1">
+        <v>40</v>
+      </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1391,16 +1601,20 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L16" s="1">
+        <v>40</v>
+      </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O16" s="1"/>
     </row>
@@ -1449,150 +1663,420 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD72A247-9488-844D-8910-8061D7C54873}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A2:E58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="str">
-        <f>""""&amp;A1&amp;""","</f>
-        <v>"Source Topic",</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="str">
-        <f t="shared" ref="B2:B15" si="0">""""&amp;A2&amp;""","</f>
-        <v>"Schema",</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="str">
-        <f t="shared" si="0"/>
-        <v>"Attribute Name",</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>"Data Type",</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>"Length",</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>"Decimal",</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>"Source To Target Mapping/Transformation Logic",</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>"Topc",</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>"Schema",</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>"Field",</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>"Data Type",</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>"Length",</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>"Decimal",</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>"Comment",</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>"CustomType",</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="12"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="12"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="12"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="12"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="12"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="12"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="12"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="12"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" s="12"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="12"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="12"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="12"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E48" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E56" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E58" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alter json object type as per xls sheet
</commit_message>
<xml_diff>
--- a/samplefile/kfk.xlsx
+++ b/samplefile/kfk.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anand/Documents/sayansi/workspaces/condaws/xlsx-json/samplefile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459E6EED-23F2-3149-A4A3-ADA000ADCACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC60690-D285-0C4F-9915-A1D34D882218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{54062B5B-119E-BD4B-B3A8-E27F027BEEC4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="2" xr2:uid="{54062B5B-119E-BD4B-B3A8-E27F027BEEC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="136">
   <si>
     <t>Source Topic</t>
   </si>
@@ -415,6 +416,36 @@
   </si>
   <si>
     <t>double</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Segment</t>
+  </si>
+  <si>
+    <t>Relation</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>asdfa</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>ZEBRA</t>
+  </si>
+  <si>
+    <t>MARS.DAP</t>
+  </si>
+  <si>
+    <t>MARS.UNIVERSE.AS</t>
   </si>
 </sst>
 </file>
@@ -573,12 +604,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -588,9 +622,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -907,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2EE713F-F4D0-1D4B-B856-52E62332C59B}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -929,14 +960,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
       <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1665,7 +1696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD72A247-9488-844D-8910-8061D7C54873}">
   <dimension ref="A2:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
@@ -1677,347 +1708,347 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="12"/>
+      <c r="B6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="12"/>
+      <c r="B10" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="9"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="9"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="9"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="9" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="12" t="s">
+      <c r="B21" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="12"/>
+      <c r="B22" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="9"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="12"/>
+      <c r="B23" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="12"/>
+      <c r="B24" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="9"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="12"/>
+      <c r="B25" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="9"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B26" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="12"/>
+      <c r="B26" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="12"/>
+      <c r="B27" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="12"/>
+      <c r="B28" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C29" s="12"/>
+      <c r="C29" s="9"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="9" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="12" t="s">
+      <c r="B33" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="12"/>
+      <c r="B34" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="9"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="12"/>
+      <c r="B35" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="9"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="12"/>
+      <c r="B36" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="9"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E46" t="s">
@@ -2077,6 +2108,205 @@
     <row r="58" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E58" t="s">
         <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2BC83BB-AFE8-4548-A31E-00B8B1C88279}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>